<commit_message>
-Fixed an issue in Regulated Taxonomy v2 where Specific yearly turnover cardinality value was invalid. The value has been changed from 1 to 1..n (ESPD-27)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.0.2-FIXED.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.0.2-FIXED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NetbeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCF6D69-0B3A-4AC0-A3B2-7BB4670A9EC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B852B3-15B3-47DD-BEAF-E62C5CBC8CC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="588" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11507" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11508" uniqueCount="427">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -13827,7 +13827,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14659,7 +14661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AW15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15680,7 +15684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AW15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16685,7 +16691,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16981,8 +16989,8 @@
         <v>0</v>
       </c>
       <c r="T5" s="19"/>
-      <c r="U5" s="19">
-        <v>1</v>
+      <c r="U5" s="97" t="s">
+        <v>20</v>
       </c>
       <c r="V5" s="23" t="s">
         <v>0</v>
@@ -21899,7 +21907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>

</xml_diff>